<commit_message>
Add bolt, nut, smps, etc
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\CoreXY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72491116-08F7-41EF-93FA-DB949F9AEE2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A351DAD3-2E17-44DC-A9B3-3E1F97802528}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7245" xr2:uid="{B2BDDEFF-1DD5-4C2F-BAB0-65787B173226}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
   <si>
     <t>150mm 2020</t>
   </si>
@@ -119,16 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mainboard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://nasspop.com/product/detail.html?product_no=149&amp;cate_no=185&amp;display_group=1</t>
-  </si>
-  <si>
-    <t>http://nasspop.com/product/list.html?cate_no=177</t>
-  </si>
-  <si>
     <t>http://nasspop.com/product/detail.html?product_no=330&amp;cate_no=72&amp;display_group=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +129,180 @@
   <si>
     <t>금액</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LM8LUU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LM8UU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=331&amp;cate_no=72&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>F623ZZ Flange Bearing</t>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=46&amp;cate_no=72&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>GT2 벨트 폭 6mm (1M)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT2 타이밍풀리 20teeth 내경 5mm 길이 16mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=118&amp;cate_no=100&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>프로파일 코너용 m5 8.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xy 아이들러용 m5 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 브라켓용 m5 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shf8용 m5 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xy 조이너용 m3 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y 캐리지용 m3 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y 캐리지용 m3 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y 캐리지용 m3 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 브라켓용 m3 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m5 8.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m5 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m5 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m5 사각너트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 일반너트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m3 나일론너트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ramps 1.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a4988 모터드라이버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=1327612</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=23966</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=23964</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=1313221</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=1322029</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34487</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34490</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34491</t>
+  </si>
+  <si>
+    <t>엔드스탑용 m3 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5sq 전선 흑색 1m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5sq 전선 적색 1m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=388&amp;cate_no=166&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=144&amp;cate_no=179&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>smps 12v 100w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=132&amp;cate_no=178&amp;display_group=1</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34324</t>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34328</t>
+  </si>
+  <si>
+    <t>m3 평와샤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=7318</t>
   </si>
 </sst>
 </file>
@@ -229,7 +393,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -246,6 +410,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1605,16 +1775,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC11325-7E82-482E-9140-E8F7F602D827}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9" style="5"/>
+    <col min="3" max="3" width="9" style="5"/>
+    <col min="4" max="4" width="9.375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1628,7 +1799,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -1663,7 +1834,7 @@
         <v>1800</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D20" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D24" si="0">B3*C3</f>
         <v>3600</v>
       </c>
       <c r="E3" t="s">
@@ -1703,7 +1874,7 @@
         <v>5600</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1744,76 +1915,100 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5">
         <v>600</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>3600</v>
+        <v>2400</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9" s="5">
+        <v>1600</v>
+      </c>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D9" si="1">B9*C9</f>
+        <v>3200</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
+        <v>650</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D10" si="2">B10*C10</f>
+        <v>10400</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1300</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" ref="D11" si="3">B11*C11</f>
+        <v>10400</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+      <c r="C12" s="5">
+        <v>500</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D12" si="4">B12*C12</f>
+        <v>1000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="0"/>
@@ -1822,10 +2017,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="0"/>
@@ -1834,10 +2029,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
@@ -1846,7 +2041,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1858,7 +2053,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1870,43 +2065,31 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="5">
-        <v>33000</v>
-      </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
-        <v>33000</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1915,14 +2098,551 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
       <c r="D21" s="5">
-        <f>SUM(D2:D20)</f>
-        <v>66160</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>33000</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>33000</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5">
+        <v>800</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>4300</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>4300</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1200</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" ref="D25" si="5">B25*C25</f>
+        <v>3600</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>16000</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" ref="D26:D38" si="6">B26*C26</f>
+        <v>16000</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>400</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="6"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>400</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="6"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29" s="5">
+        <v>80</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="6"/>
+        <v>1920</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30" s="5">
+        <v>80</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="6"/>
+        <v>960</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31" s="5">
+        <v>80</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="6"/>
+        <v>640</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>50</v>
+      </c>
+      <c r="C32" s="5">
+        <v>40</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33" s="7">
+        <v>37</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="6"/>
+        <v>1110</v>
+      </c>
+      <c r="E33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" s="7">
+        <v>49</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="6"/>
+        <v>1470</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35" s="7">
+        <v>56</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="6"/>
+        <v>1120</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36">
+        <v>50</v>
+      </c>
+      <c r="C36" s="7">
+        <v>8</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="E36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37">
+        <v>40</v>
+      </c>
+      <c r="C37" s="7">
+        <v>15</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38" s="7">
+        <v>10</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="E38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D39" s="5">
+        <f>SUM(D2:D38)</f>
+        <v>126480</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44" s="5">
+        <v>80</v>
+      </c>
+      <c r="E44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45" s="5">
+        <v>80</v>
+      </c>
+      <c r="E45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46" s="5">
+        <v>80</v>
+      </c>
+      <c r="E46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>50</v>
+      </c>
+      <c r="C47" s="5">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <v>12</v>
+      </c>
+      <c r="C48" s="5">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>19</v>
+      </c>
+      <c r="C49" s="5">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" s="5">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>50</v>
+      </c>
+      <c r="C52" s="5">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>40</v>
+      </c>
+      <c r="C53" s="5">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54" s="5">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1936,7 +2656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0AA720-F6B8-4731-935B-E8818E0D11E9}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
F623ZZ Flange Bearing + 4 GT2 Belt -2
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\CoreXY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A8A8B-9327-49C2-BCA2-78A74CADE1DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BF8CA0-7620-4EDF-A01F-FE1064ABE640}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7245" xr2:uid="{B2BDDEFF-1DD5-4C2F-BAB0-65787B173226}"/>
   </bookViews>
@@ -1780,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC11325-7E82-482E-9140-E8F7F602D827}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1957,14 +1957,14 @@
         <v>33</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>650</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" ref="D10" si="2">B10*C10</f>
-        <v>10400</v>
+        <v>13000</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
@@ -1975,14 +1975,14 @@
         <v>35</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5">
         <v>1300</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" ref="D11" si="3">B11*C11</f>
-        <v>10400</v>
+        <v>7800</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Change motor bracket, update BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\CoreXY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BF8CA0-7620-4EDF-A01F-FE1064ABE640}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C98C65-A4EA-495C-B070-5171C3766A6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7245" xr2:uid="{B2BDDEFF-1DD5-4C2F-BAB0-65787B173226}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="85">
   <si>
     <t>150mm 2020</t>
   </si>
@@ -167,10 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>모터 브라켓용 m5 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>shf8용 m5 15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -303,6 +299,34 @@
   </si>
   <si>
     <t>http://www.devicemart.co.kr/goods/view?no=7318</t>
+  </si>
+  <si>
+    <t>금속 모터브라켓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m4 사각너트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m4 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 브라켓용 m4 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/goods/view?no=34496</t>
+  </si>
+  <si>
+    <t>https://smartstore.naver.com/3dprinter/products/273464690</t>
+  </si>
+  <si>
+    <t>https://smartstore.naver.com/3dprinter/products/269715459</t>
+  </si>
+  <si>
+    <t>http://nasspop.com/product/detail.html?product_no=43&amp;cate_no=186&amp;display_group=1</t>
   </si>
 </sst>
 </file>
@@ -1778,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC11325-7E82-482E-9140-E8F7F602D827}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1837,7 +1861,7 @@
         <v>1800</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D24" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
         <v>3600</v>
       </c>
       <c r="E3" t="s">
@@ -2048,7 +2072,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2060,7 +2084,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2072,7 +2096,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2084,7 +2108,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2096,62 +2120,74 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1500</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D20" si="5">B20*C20</f>
+        <v>3000</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
+      <c r="C21" s="5">
+        <v>33000</v>
+      </c>
       <c r="D21" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33000</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="5">
-        <v>33000</v>
+        <v>800</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>1600</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>800</v>
+        <v>4300</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>4300</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2159,14 +2195,14 @@
         <v>57</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" s="5">
-        <v>4300</v>
+        <v>1200</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="0"/>
-        <v>4300</v>
+        <f t="shared" ref="D24" si="6">B24*C24</f>
+        <v>3600</v>
       </c>
       <c r="E24" t="s">
         <v>70</v>
@@ -2174,38 +2210,38 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>1200</v>
+        <v>16000</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" ref="D25" si="5">B25*C25</f>
-        <v>3600</v>
+        <f t="shared" ref="D25:D39" si="7">B25*C25</f>
+        <v>16000</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="5">
-        <v>16000</v>
+        <v>400</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" ref="D26:D38" si="6">B26*C26</f>
-        <v>16000</v>
+        <f t="shared" si="7"/>
+        <v>800</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2219,27 +2255,30 @@
         <v>400</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>800</v>
+      </c>
+      <c r="E27" s="8">
+        <f>SUM(D20:D27)</f>
+        <v>63100</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C28" s="5">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="6"/>
-        <v>800</v>
-      </c>
-      <c r="E28" s="8">
-        <f>SUM(D22:D27)</f>
-        <v>59300</v>
+        <f t="shared" si="7"/>
+        <v>2240</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2247,14 +2286,14 @@
         <v>47</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C29" s="5">
         <v>80</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="6"/>
-        <v>2240</v>
+        <f t="shared" si="7"/>
+        <v>1280</v>
       </c>
       <c r="E29" t="s">
         <v>61</v>
@@ -2265,14 +2304,14 @@
         <v>48</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C30" s="5">
         <v>80</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="6"/>
-        <v>1280</v>
+        <f t="shared" si="7"/>
+        <v>960</v>
       </c>
       <c r="E30" t="s">
         <v>62</v>
@@ -2280,38 +2319,38 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C31" s="5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="6"/>
-        <v>960</v>
+        <f t="shared" si="7"/>
+        <v>2400</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B32">
-        <v>60</v>
-      </c>
-      <c r="C32" s="5">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="C32" s="7">
+        <v>37</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="6"/>
-        <v>2400</v>
+        <f t="shared" si="7"/>
+        <v>1110</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -2322,11 +2361,11 @@
         <v>30</v>
       </c>
       <c r="C33" s="7">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="6"/>
-        <v>1110</v>
+        <f t="shared" si="7"/>
+        <v>1470</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -2337,14 +2376,14 @@
         <v>51</v>
       </c>
       <c r="B34">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C34" s="7">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="6"/>
-        <v>1470</v>
+        <f t="shared" si="7"/>
+        <v>1120</v>
       </c>
       <c r="E34" t="s">
         <v>65</v>
@@ -2352,20 +2391,20 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C35" s="7">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="6"/>
-        <v>1120</v>
+        <f t="shared" si="7"/>
+        <v>400</v>
       </c>
       <c r="E35" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2373,14 +2412,14 @@
         <v>55</v>
       </c>
       <c r="B36">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C36" s="7">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="6"/>
-        <v>400</v>
+        <f t="shared" si="7"/>
+        <v>600</v>
       </c>
       <c r="E36" t="s">
         <v>74</v>
@@ -2388,48 +2427,80 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B37">
         <v>40</v>
       </c>
       <c r="C37" s="7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="6"/>
-        <v>600</v>
+        <f t="shared" si="7"/>
+        <v>400</v>
       </c>
       <c r="E37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B38">
-        <v>40</v>
-      </c>
-      <c r="C38" s="7">
         <v>10</v>
       </c>
+      <c r="C38" s="5">
+        <v>37</v>
+      </c>
       <c r="D38" s="5">
-        <f t="shared" si="6"/>
-        <v>400</v>
+        <f t="shared" si="7"/>
+        <v>370</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5">
+        <v>30</v>
+      </c>
       <c r="D39" s="5">
-        <f>SUM(D2:D38)</f>
-        <v>127840</v>
-      </c>
-      <c r="E39" s="8">
-        <f>SUM(D29:D38)</f>
-        <v>11980</v>
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D40" s="5">
+        <f>SUM(D2:D39)</f>
+        <v>131510</v>
+      </c>
+      <c r="E40" s="8">
+        <f>SUM(D28:D39)</f>
+        <v>12650</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43" s="5">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -2437,7 +2508,7 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C44" s="5">
         <v>80</v>
@@ -2451,7 +2522,7 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C45" s="5">
         <v>80</v>
@@ -2462,30 +2533,30 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C46" s="5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B47">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C47" s="5">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -2493,10 +2564,10 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C48" s="5">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E48" t="s">
         <v>64</v>
@@ -2507,10 +2578,10 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C49" s="5">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
         <v>65</v>
@@ -2521,21 +2592,21 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>8</v>
-      </c>
-      <c r="C50" s="5">
-        <v>30</v>
-      </c>
-      <c r="E50" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C51" s="5">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2543,10 +2614,10 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C52" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
         <v>74</v>
@@ -2554,59 +2625,59 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B53">
         <v>40</v>
       </c>
       <c r="C53" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B54">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C54" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55">
         <v>10</v>
       </c>
-      <c r="E54" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56">
-        <v>24</v>
+      <c r="C55" s="5">
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B59">
         <v>8</v>
@@ -2614,7 +2685,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -2622,41 +2693,49 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B61">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B63">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66">
         <v>4</v>
       </c>
     </row>

</xml_diff>